<commit_message>
testing the output of both an optimized schedule and a schedule that outputs all availabilities for every given hour.
</commit_message>
<xml_diff>
--- a/workersAvailability.xlsx
+++ b/workersAvailability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amulek/Desktop/chemStores_scheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332547CB-9B55-8748-B8E9-C62680B0A337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241506F5-012A-564F-AE84-C11A6AEC1422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,49 +78,49 @@
     <t>11,17</t>
   </si>
   <si>
-    <t>Thomas</t>
-  </si>
-  <si>
-    <t>Brandon</t>
-  </si>
-  <si>
-    <t>Lynsey</t>
-  </si>
-  <si>
-    <t>Makayla</t>
-  </si>
-  <si>
-    <t>Chloe</t>
-  </si>
-  <si>
     <t>12,16</t>
   </si>
   <si>
-    <t>Andrew</t>
-  </si>
-  <si>
-    <t>Amulek</t>
-  </si>
-  <si>
-    <t>Zach</t>
-  </si>
-  <si>
     <t>10,13</t>
   </si>
   <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Levi</t>
-  </si>
-  <si>
-    <t>Eleanor</t>
-  </si>
-  <si>
     <t>10,14</t>
   </si>
   <si>
     <t>10,15</t>
+  </si>
+  <si>
+    <t>worker 1</t>
+  </si>
+  <si>
+    <t>worker 2</t>
+  </si>
+  <si>
+    <t>worker 3</t>
+  </si>
+  <si>
+    <t>worker 4</t>
+  </si>
+  <si>
+    <t>worker 5</t>
+  </si>
+  <si>
+    <t>worker 6</t>
+  </si>
+  <si>
+    <t>worker 7</t>
+  </si>
+  <si>
+    <t>worker 8</t>
+  </si>
+  <si>
+    <t>worker 9</t>
+  </si>
+  <si>
+    <t>worker 10</t>
+  </si>
+  <si>
+    <t>worker 11</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3"/>
+      <selection pane="topRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -547,7 +547,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -711,34 +711,34 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="K6" t="s">
         <v>13</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -793,7 +793,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>11</v>
@@ -834,28 +834,28 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
         <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="I9" t="s">
         <v>13</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>12</v>
@@ -916,7 +916,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -957,7 +957,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>9</v>

</xml_diff>